<commit_message>
Second commit after updates added: PageUtility SubcategoryClass ManageUserClass EdittestcaseinCategoryClass
</commit_message>
<xml_diff>
--- a/SeleniumAutomationproject/src/test/resources/Testdata.xlsx
+++ b/SeleniumAutomationproject/src/test/resources/Testdata.xlsx
@@ -4,19 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="Category" sheetId="2" r:id="rId2"/>
     <sheet name="NewsSearch" sheetId="3" r:id="rId3"/>
+    <sheet name="Subcategory" sheetId="4" r:id="rId4"/>
+    <sheet name="ManageUsers" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
   <si>
     <t>username</t>
   </si>
@@ -39,9 +41,6 @@
     <t>Bread983241</t>
   </si>
   <si>
-    <t>Bread983242</t>
-  </si>
-  <si>
     <t>Bread983243</t>
   </si>
   <si>
@@ -57,7 +56,37 @@
     <t>Create</t>
   </si>
   <si>
-    <t>R</t>
+    <t>admin123</t>
+  </si>
+  <si>
+    <t>admin435</t>
+  </si>
+  <si>
+    <t>test456</t>
+  </si>
+  <si>
+    <t>news</t>
+  </si>
+  <si>
+    <t>SubcategoryName</t>
+  </si>
+  <si>
+    <t>AddToyForTest_2190876</t>
+  </si>
+  <si>
+    <t>CategoryEdited452</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>testfordemo503</t>
+  </si>
+  <si>
+    <t>saumya1993</t>
   </si>
 </sst>
 </file>
@@ -396,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -444,6 +473,22 @@
         <v>4</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -453,13 +498,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" customWidth="1"/>
+    <col min="1" max="1" width="17.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
@@ -474,22 +519,22 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -501,8 +546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -512,22 +557,85 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.21875" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fourth commit Added: config file under src/main/resources added chaining removed hard coded values added Wait formatted code
</commit_message>
<xml_diff>
--- a/SeleniumAutomationproject/src/test/resources/Testdata.xlsx
+++ b/SeleniumAutomationproject/src/test/resources/Testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
   <si>
     <t>username</t>
   </si>
@@ -87,6 +87,18 @@
   </si>
   <si>
     <t>saumya1993</t>
+  </si>
+  <si>
+    <t>UserType</t>
+  </si>
+  <si>
+    <t>Staff</t>
+  </si>
+  <si>
+    <t>Dropdownvalue</t>
+  </si>
+  <si>
+    <t>Toys</t>
   </si>
 </sst>
 </file>
@@ -498,7 +510,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -582,10 +594,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -593,14 +605,20 @@
     <col min="1" max="1" width="22.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -610,10 +628,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -622,20 +640,26 @@
     <col min="2" max="2" width="14.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>19</v>
       </c>
       <c r="B1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>22</v>
       </c>
       <c r="B2" t="s">
         <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>